<commit_message>
yet another update of the list
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -16739,7 +16739,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Di Giacomo, Matteo</t>
+          <t>Di Giacomo, Matteo</t>
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -23686,7 +23686,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-54</t>
+          <t>F4E-OMF-1159-01-01-125</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -50972,13 +50972,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF5D33C-7633-40DE-98C5-9D86E69A4FB5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E8C719-C8BC-48C8-88E1-4283A5F70F24}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADAAA974-85EC-4255-B458-98FF1A5CBB2A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28922ACF-8DC9-485A-8226-30D8E8BDF380}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF56BF68-60F1-42DA-8A4F-C780AE2AD020}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1A58F7E-80A9-4E24-A4BC-8F33093E837C}"/>
 </file>
</xml_diff>

<commit_message>
List of employees update
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -9546,7 +9546,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Juan Martín Val</t>
+          <t>Juan Martín</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -18765,7 +18765,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>https://idm.f4e.europa.eu/default.aspx?uid=39MJUL</t>
+          <t>https://idm.f4e.europa.eu/?uid=39H73P</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -19216,89 +19216,85 @@
       <c r="BR75" t="inlineStr"/>
       <c r="BS75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00666</t>
+          <t>ATG-EU-RP-PC-F4E-25-00667</t>
         </is>
       </c>
       <c r="BT75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00667</t>
+          <t>ATG-EU-RP-PC-F4E-25-00668</t>
         </is>
       </c>
       <c r="BU75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00668</t>
+          <t>ATG-EU-RP-PC-F4E-25-00669</t>
         </is>
       </c>
       <c r="BV75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00669</t>
+          <t>ATG-EU-RP-PC-F4E-25-00670</t>
         </is>
       </c>
       <c r="BW75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00670</t>
+          <t>ATG-EU-RP-PC-F4E-25-00671</t>
         </is>
       </c>
       <c r="BX75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00671</t>
+          <t>ATG-EU-RP-PC-F4E-25-00672</t>
         </is>
       </c>
       <c r="BY75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00672</t>
+          <t>ATG-EU-RP-PC-F4E-25-00673</t>
         </is>
       </c>
       <c r="BZ75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00673</t>
+          <t>ATG-EU-RP-PC-F4E-25-00674</t>
         </is>
       </c>
       <c r="CA75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00674</t>
+          <t>ATG-EU-RP-PC-F4E-25-00675</t>
         </is>
       </c>
       <c r="CB75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00675</t>
+          <t>ATG-EU-RP-PC-F4E-25-00676</t>
         </is>
       </c>
       <c r="CC75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00676</t>
+          <t>ATG-EU-RP-PC-F4E-25-00677</t>
         </is>
       </c>
       <c r="CD75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00677</t>
+          <t>ATG-EU-RP-PC-F4E-25-00678</t>
         </is>
       </c>
       <c r="CE75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00678</t>
+          <t>ATG-EU-RP-PC-F4E-25-00679</t>
         </is>
       </c>
       <c r="CF75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00679</t>
+          <t>ATG-EU-RP-PC-F4E-25-00680</t>
         </is>
       </c>
       <c r="CG75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00680</t>
+          <t>ATG-EU-RP-PC-F4E-25-00681</t>
         </is>
       </c>
       <c r="CH75" t="inlineStr">
         <is>
-          <t>ATG-EU-RP-PC-F4E-25-00681</t>
-        </is>
-      </c>
-      <c r="CI75" t="inlineStr">
-        <is>
           <t>ATG-EU-RP-PC-F4E-25-00682</t>
         </is>
       </c>
+      <c r="CI75" t="inlineStr"/>
       <c r="CJ75" t="inlineStr"/>
       <c r="CK75" t="inlineStr"/>
       <c r="CL75" t="inlineStr"/>
@@ -20298,7 +20294,7 @@
       <c r="R79" t="inlineStr"/>
       <c r="S79" t="inlineStr"/>
       <c r="T79" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U79" t="inlineStr"/>
       <c r="V79" t="inlineStr"/>
@@ -20846,7 +20842,7 @@
       <c r="R81" t="inlineStr"/>
       <c r="S81" t="inlineStr"/>
       <c r="T81" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U81" t="inlineStr"/>
       <c r="V81" t="inlineStr"/>
@@ -21164,7 +21160,7 @@
       <c r="R82" t="inlineStr"/>
       <c r="S82" t="inlineStr"/>
       <c r="T82" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
@@ -21482,7 +21478,7 @@
       <c r="R83" t="inlineStr"/>
       <c r="S83" t="inlineStr"/>
       <c r="T83" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr"/>
@@ -21780,7 +21776,7 @@
       <c r="R84" t="inlineStr"/>
       <c r="S84" t="inlineStr"/>
       <c r="T84" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U84" t="inlineStr"/>
       <c r="V84" t="inlineStr"/>
@@ -22416,7 +22412,7 @@
       <c r="R86" t="inlineStr"/>
       <c r="S86" t="inlineStr"/>
       <c r="T86" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U86" t="inlineStr"/>
       <c r="V86" t="inlineStr"/>
@@ -22682,7 +22678,7 @@
       <c r="R87" t="inlineStr"/>
       <c r="S87" t="inlineStr"/>
       <c r="T87" t="n">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="U87" t="inlineStr"/>
       <c r="V87" t="inlineStr"/>
@@ -23000,7 +22996,7 @@
       <c r="R88" t="inlineStr"/>
       <c r="S88" t="inlineStr"/>
       <c r="T88" t="n">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="U88" t="inlineStr"/>
       <c r="V88" t="inlineStr"/>
@@ -23222,7 +23218,7 @@
       <c r="R89" t="inlineStr"/>
       <c r="S89" t="inlineStr"/>
       <c r="T89" t="n">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
@@ -23758,7 +23754,7 @@
       <c r="R91" t="inlineStr"/>
       <c r="S91" t="inlineStr"/>
       <c r="T91" t="n">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="U91" t="inlineStr"/>
       <c r="V91" t="inlineStr"/>
@@ -24326,7 +24322,7 @@
       <c r="R93" t="inlineStr"/>
       <c r="S93" t="inlineStr"/>
       <c r="T93" t="n">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
@@ -24644,7 +24640,7 @@
       <c r="R94" t="inlineStr"/>
       <c r="S94" t="inlineStr"/>
       <c r="T94" t="n">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="U94" t="inlineStr"/>
       <c r="V94" t="inlineStr"/>
@@ -26129,7 +26125,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Miguel Garcia Lopez Astilleros</t>
+          <t>Miguel García López Astilleros</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -26422,12 +26418,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-25</t>
+          <t>F4E-OMF-1159-01-01-129</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Bernardo Balleste</t>
+          <t>Bernardo Ballesté</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -26736,12 +26732,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-25</t>
+          <t>F4E-OMF-1159-01-01-129</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Marc Mari Gimeno</t>
+          <t>Marc Marí Gimeno</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -27050,12 +27046,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-26</t>
+          <t>F4E-OMF-1159-01-01-135</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Jose Antonio Soto Sanz</t>
+          <t>José Antonio Soto Sanz</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -27595,7 +27591,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Carlos Rodriguez Hevia</t>
+          <t>Carlos Rodríguez Hevia</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -28139,7 +28135,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Jordi Jimenez</t>
+          <t>Jordi Jiménez</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -28436,12 +28432,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-39</t>
+          <t>F4E-OMF-1159-01-01-138</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Domingo Martinez Santiago</t>
+          <t>Domingo Martínez Santiago</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -28746,12 +28742,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-39</t>
+          <t>F4E-OMF-1159-01-01-138</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Victor Carrero Gonzalez</t>
+          <t>Víctor Carrero González</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -29048,7 +29044,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-42</t>
+          <t>F4E-OMF-1159-01-01-143</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -29358,12 +29354,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-51</t>
+          <t>F4E-OMF-1159-01-01-140</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Juan Carlos Salgado Perez</t>
+          <t>Juan Carlos Salgado Pérez</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -29668,7 +29664,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-52</t>
+          <t>F4E-OMF-1159-01-01-127</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -30216,7 +30212,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-66</t>
+          <t>F4E-OMF-1159-01-01-136</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -32768,7 +32764,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-34</t>
+          <t>F4E-OMF-1159-01-01-136</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -33063,89 +33059,97 @@
           <t>ATG-EU-RP-PC-F4E-24-09571</t>
         </is>
       </c>
-      <c r="BN125" t="inlineStr">
+      <c r="BN125" t="inlineStr"/>
+      <c r="BO125" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-24-09570</t>
+        </is>
+      </c>
+      <c r="BP125" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-24-09571</t>
+        </is>
+      </c>
+      <c r="BQ125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09572</t>
         </is>
       </c>
-      <c r="BO125" t="inlineStr">
+      <c r="BR125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09573</t>
         </is>
       </c>
-      <c r="BP125" t="inlineStr">
+      <c r="BS125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09574</t>
         </is>
       </c>
-      <c r="BQ125" t="inlineStr">
+      <c r="BT125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09575</t>
         </is>
       </c>
-      <c r="BR125" t="inlineStr">
+      <c r="BU125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09576</t>
         </is>
       </c>
-      <c r="BS125" t="inlineStr">
+      <c r="BV125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09577</t>
         </is>
       </c>
-      <c r="BT125" t="inlineStr">
+      <c r="BW125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09578</t>
         </is>
       </c>
-      <c r="BU125" t="inlineStr">
+      <c r="BX125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09579</t>
         </is>
       </c>
-      <c r="BV125" t="inlineStr">
+      <c r="BY125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09580</t>
         </is>
       </c>
-      <c r="BW125" t="inlineStr">
+      <c r="BZ125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09581</t>
         </is>
       </c>
-      <c r="BX125" t="inlineStr">
+      <c r="CA125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09582</t>
         </is>
       </c>
-      <c r="BY125" t="inlineStr">
+      <c r="CB125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09583</t>
         </is>
       </c>
-      <c r="BZ125" t="inlineStr">
+      <c r="CC125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09584</t>
         </is>
       </c>
-      <c r="CA125" t="inlineStr">
+      <c r="CD125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09585</t>
         </is>
       </c>
-      <c r="CB125" t="inlineStr">
+      <c r="CE125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09586</t>
         </is>
       </c>
-      <c r="CC125" t="inlineStr">
+      <c r="CF125" t="inlineStr">
         <is>
           <t>ATG-EU-RP-PC-F4E-24-09587</t>
         </is>
       </c>
-      <c r="CD125" t="inlineStr"/>
-      <c r="CE125" t="inlineStr"/>
-      <c r="CF125" t="inlineStr"/>
       <c r="CG125" t="inlineStr"/>
       <c r="CH125" t="inlineStr"/>
       <c r="CI125" t="inlineStr"/>
@@ -45818,7 +45822,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t xml:space="preserve">F4E-OMF-1159-01-01-130 </t>
+          <t>F4E-OMF-1159-01-01-130</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -46060,7 +46064,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t xml:space="preserve">F4E-OMF-1159-01-01-119 </t>
+          <t>F4E-OMF-1159-01-01-119</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -50498,45 +50502,129 @@
       <c r="BP197" t="inlineStr"/>
       <c r="BQ197" t="inlineStr"/>
       <c r="BR197" t="inlineStr"/>
-      <c r="BS197" t="inlineStr"/>
-      <c r="BT197" t="inlineStr"/>
-      <c r="BU197" t="inlineStr"/>
-      <c r="BV197" t="inlineStr"/>
-      <c r="BW197" t="inlineStr"/>
-      <c r="BX197" t="inlineStr"/>
-      <c r="BY197" t="inlineStr"/>
-      <c r="BZ197" t="inlineStr"/>
-      <c r="CA197" t="inlineStr"/>
-      <c r="CB197" t="inlineStr"/>
-      <c r="CC197" t="inlineStr"/>
-      <c r="CD197" t="inlineStr"/>
-      <c r="CE197" t="inlineStr"/>
-      <c r="CF197" t="inlineStr"/>
-      <c r="CG197" t="inlineStr"/>
-      <c r="CH197" t="inlineStr"/>
-      <c r="CI197" t="inlineStr"/>
-      <c r="CJ197" t="inlineStr"/>
+      <c r="BS197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01261</t>
+        </is>
+      </c>
+      <c r="BT197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01262</t>
+        </is>
+      </c>
+      <c r="BU197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01263</t>
+        </is>
+      </c>
+      <c r="BV197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01264</t>
+        </is>
+      </c>
+      <c r="BW197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01265</t>
+        </is>
+      </c>
+      <c r="BX197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01266</t>
+        </is>
+      </c>
+      <c r="BY197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01267</t>
+        </is>
+      </c>
+      <c r="BZ197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01268</t>
+        </is>
+      </c>
+      <c r="CA197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01269</t>
+        </is>
+      </c>
+      <c r="CB197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01270</t>
+        </is>
+      </c>
+      <c r="CC197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01271</t>
+        </is>
+      </c>
+      <c r="CD197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01272</t>
+        </is>
+      </c>
+      <c r="CE197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01273</t>
+        </is>
+      </c>
+      <c r="CF197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01274</t>
+        </is>
+      </c>
+      <c r="CG197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01275</t>
+        </is>
+      </c>
+      <c r="CH197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01276</t>
+        </is>
+      </c>
+      <c r="CI197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01277</t>
+        </is>
+      </c>
+      <c r="CJ197" t="inlineStr">
+        <is>
+          <t>ATG-EU-RP-PC-F4E-25-01278</t>
+        </is>
+      </c>
       <c r="CK197" t="inlineStr"/>
       <c r="CL197" t="inlineStr"/>
       <c r="CM197" t="inlineStr"/>
       <c r="CN197" t="inlineStr"/>
     </row>
     <row r="198">
-      <c r="A198" t="inlineStr"/>
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>F4E-OMF-1159-01-01-159</t>
+        </is>
+      </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Matteo</t>
+          <t>Matteo Faoro</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
       <c r="D198" t="inlineStr"/>
       <c r="E198" t="inlineStr"/>
-      <c r="F198" t="inlineStr"/>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="inlineStr"/>
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr"/>
-      <c r="K198" t="inlineStr"/>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>Naka</t>
+        </is>
+      </c>
       <c r="L198" t="inlineStr"/>
       <c r="M198" t="inlineStr"/>
       <c r="N198" t="inlineStr"/>
@@ -50620,21 +50708,33 @@
       <c r="CN198" t="inlineStr"/>
     </row>
     <row r="199">
-      <c r="A199" t="inlineStr"/>
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>F4E-OMF-1159-01-01-159</t>
+        </is>
+      </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Michele</t>
+          <t>Michele Piccirelli</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
       <c r="D199" t="inlineStr"/>
       <c r="E199" t="inlineStr"/>
-      <c r="F199" t="inlineStr"/>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="inlineStr"/>
       <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr"/>
-      <c r="K199" t="inlineStr"/>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>Naka</t>
+        </is>
+      </c>
       <c r="L199" t="inlineStr"/>
       <c r="M199" t="inlineStr"/>
       <c r="N199" t="inlineStr"/>
@@ -50972,13 +51072,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E8C719-C8BC-48C8-88E1-4283A5F70F24}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955D5721-7C79-4251-97C4-6142E45E2903}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28922ACF-8DC9-485A-8226-30D8E8BDF380}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353EB616-4B36-4EF6-AD9E-F2A7D546ECF3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1A58F7E-80A9-4E24-A4BC-8F33093E837C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8171EE48-A152-4D00-B607-DFDC20B73DAA}"/>
 </file>
</xml_diff>

<commit_message>
Update List of Employees 06052025
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -50089,7 +50089,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Naim Forghani</t>
+          <t>Naim Forghani Teruel</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -50112,12 +50112,12 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Naim Forghani</t>
+          <t>Naim Forghani Teruel</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Forghani, Naim</t>
+          <t>Forghani Teruel, Naim</t>
         </is>
       </c>
       <c r="I196" t="inlineStr"/>
@@ -52724,13 +52724,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AE02ACA-023E-4078-9F7A-6FF42EA5DBD4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F7324BF-27FD-41D2-99E7-AE8C7C77663A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0CF9B9-ACE3-4154-994A-7BE8198FADBE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{615CB113-DDBA-4650-B939-5C6E9282A9B9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8597F362-8C8C-4582-9453-1801AB67241A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2DBCF89-9D3F-4274-9585-AE23A1C7B802}"/>
 </file>
</xml_diff>

<commit_message>
Update of list of employees 2
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -9741,7 +9741,11 @@
           <t>Cristo Peregrin</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>B - Senior Expert Mech. Eng.</t>
+        </is>
+      </c>
       <c r="E35" s="2" t="n">
         <v>45748</v>
       </c>
@@ -9943,7 +9947,11 @@
           <t>Cristo Peregrin</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>D - Senior Expert Elect. Eng.</t>
+        </is>
+      </c>
       <c r="E36" s="2" t="n">
         <v>45748</v>
       </c>
@@ -9970,7 +9978,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Barcleona</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
@@ -52966,13 +52974,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCFCCC2-72EE-4498-B228-877E1A4C8F87}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F825FAF-B487-42AD-AEC0-42F1EDDF8CF6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA18564-20C5-45A1-A996-4C7D09D1DC33}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A932482A-27CD-42F7-924D-1D44D8385272}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BF8FC59-94DC-49AB-81A9-853CED63D41D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E414C1-2DB2-4D33-9196-0402EA203815}"/>
 </file>
</xml_diff>

<commit_message>
List of Employees 03/06
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -9555,7 +9555,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Martín, Juan </t>
+          <t>Martín, Juan</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -34387,7 +34387,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Rodrigues, Alexandra</t>
+          <t>Rodrigues, Maria Alexandra</t>
         </is>
       </c>
       <c r="I132" t="inlineStr"/>
@@ -48836,12 +48836,20 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="G191" t="inlineStr"/>
-      <c r="H191" t="inlineStr"/>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>Francesc García</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Garcia, Francesc</t>
+        </is>
+      </c>
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr">
         <is>
-          <t>https://idm.f4e.europa.eu/?uid=35KZL3</t>
+          <t>https://idm.f4e.europa.eu/?uid=3C55AH</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -52974,13 +52982,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F825FAF-B487-42AD-AEC0-42F1EDDF8CF6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AF5AB7-5DA1-4222-8338-5EA35E3AA077}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A932482A-27CD-42F7-924D-1D44D8385272}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CEAA81-E03E-4675-B0B0-C17530658747}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E414C1-2DB2-4D33-9196-0402EA203815}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A4C32C8-997F-4078-A22E-689E8F582354}"/>
 </file>
</xml_diff>

<commit_message>
update of list of employees 05/06
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -3030,12 +3030,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Jose Duo</t>
+          <t>Jose Ignacio Duo</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Duo, Jose</t>
+          <t>Duo, José</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -9733,7 +9733,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>José Vargas</t>
+          <t>Jose Vargas</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -9756,12 +9756,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>José Vargas</t>
+          <t>Jose Vargas</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Vargas, José</t>
+          <t>Vargas, Jose</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -51988,7 +51988,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-80</t>
+          <t>F4E-OMF-1159-01-01-144</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -52982,13 +52982,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AF5AB7-5DA1-4222-8338-5EA35E3AA077}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983F939C-A540-48B8-BF24-7525B2423488}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CEAA81-E03E-4675-B0B0-C17530658747}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B4C4C2-5A6F-4362-AC6F-BC5008F40D25}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A4C32C8-997F-4078-A22E-689E8F582354}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAE20EC5-2192-4412-855A-3AED22D13A93}"/>
 </file>
</xml_diff>

<commit_message>
update list employees 0506
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -50966,7 +50966,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Shoichi Mizumaki</t>
+          <t>Mizumaki Shoichi</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -52982,13 +52982,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983F939C-A540-48B8-BF24-7525B2423488}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B98396-DCAA-41D0-9C76-BE63F971F937}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B4C4C2-5A6F-4362-AC6F-BC5008F40D25}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3312479-EC71-476B-9DE0-BC336989E6EB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAE20EC5-2192-4412-855A-3AED22D13A93}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE330DDB-C00C-46B8-A835-389B7272C9F4}"/>
 </file>
</xml_diff>

<commit_message>
update list employees 0606
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -51784,7 +51784,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>F4E-OMF-1159-01-01-142</t>
+          <t>F4E-OMF-1159-01-01-131</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -51817,7 +51817,7 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Cambria, Chiara</t>
+          <t>Cambria Zurro, Chiara</t>
         </is>
       </c>
       <c r="I204" t="inlineStr"/>
@@ -52982,13 +52982,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B98396-DCAA-41D0-9C76-BE63F971F937}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB30BEC-EDFA-4E79-80F4-A744051CFA8F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3312479-EC71-476B-9DE0-BC336989E6EB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F945EBD6-AD38-4A7D-AB0D-F712663ABA95}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE330DDB-C00C-46B8-A835-389B7272C9F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F99C66CC-EDBC-43FA-A336-78F1C9E933C3}"/>
 </file>
</xml_diff>

<commit_message>
Update list of employees 1006
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -23723,7 +23723,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Cretu, Marian</t>
+          <t>Cretu, Marian-Florentin</t>
         </is>
       </c>
       <c r="I92" t="inlineStr"/>
@@ -52982,13 +52982,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB30BEC-EDFA-4E79-80F4-A744051CFA8F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABEF5742-5A98-453E-A76E-7B2685A60E0F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F945EBD6-AD38-4A7D-AB0D-F712663ABA95}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0768E166-DA02-4F16-9AFC-7A07EEAE30C0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F99C66CC-EDBC-43FA-A336-78F1C9E933C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98ADF764-78E9-4F3D-A366-CBEB31DF0916}"/>
 </file>
</xml_diff>

<commit_message>
update list of employees 04/07
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -36048,7 +36048,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t xml:space="preserve">F4E-OMF-1159-01-01-164 </t>
+          <t>F4E-OMF-1159-01-01-164</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -36508,13 +36508,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE25B42A-B949-4D30-B20E-274550E94D1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69BC99F-EF83-45D9-AE30-FE4802D8486C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2358AF14-32E7-4EA7-930E-73B75BBDA771}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8F347E-A7F3-45D5-A8E9-EB46C3B6EC1B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E2103D-83D7-400B-9F38-01A864F30ADC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47465075-3A2C-4D45-AE4E-3C9C64C8ED17}"/>
 </file>
</xml_diff>

<commit_message>
update list of employees 06/08
</commit_message>
<xml_diff>
--- a/LIST OF EMPLOYEES.xlsx
+++ b/LIST OF EMPLOYEES.xlsx
@@ -33726,7 +33726,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Sevil de Veer</t>
+          <t>Juan Torre</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -37223,7 +37223,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Morales, Juan Carlos</t>
+          <t>Morales, Juancarlos</t>
         </is>
       </c>
       <c r="I137" t="inlineStr"/>
@@ -37461,7 +37461,7 @@
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://idm.f4e.europa.eu/?uid=3B9QHR </t>
+          <t>https://idm.f4e.europa.eu//?uid=3CLQZZ</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -37877,22 +37877,22 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
+    <TaxCatchAll xmlns="e82ac38b-faea-4ea8-bff9-d97ba262ba29" xsi:nil="true"/>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="23d0c39d-f35f-4b16-8d90-ad825ca80df4">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e82ac38b-faea-4ea8-bff9-d97ba262ba29" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54FD1BBB-A2D8-4A18-A2F5-F7832B42843D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6C1CD51-4310-427D-857F-3E106636BE4F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07D8B4DD-E0B9-4553-BBED-E7894672DA5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B3E190-384B-42F4-8EBE-7307B3136176}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60D4DA39-ADD0-4DB4-A238-5444EC886BC0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52FC8765-ADE7-48E3-B2AC-CA2A028F0190}"/>
 </file>
</xml_diff>